<commit_message>
Notendagreining aðrir yfirmenn komnir inn
</commit_message>
<xml_diff>
--- a/notendagreining.xlsx
+++ b/notendagreining.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gudmundur\Dropbox\Tölvunarfræði\Verk1\hópverk\verklegtnamskeid1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patti\Desktop\Verk nám\verklegtnamskeid1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9300DFDE-8253-4C5C-B30B-3922BCFA425F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B26F26-0482-425E-96F5-E591AC6349EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Greining Notendahópa / User Group Analysis</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Framhaldsmenntun</t>
   </si>
   <si>
-    <t>reynslu og góða þekkingu</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2 - 3</t>
   </si>
   <si>
@@ -135,28 +132,22 @@
     <t>Mjög mikilvægur</t>
   </si>
   <si>
-    <t>Chuck Norris</t>
-  </si>
-  <si>
-    <t>á ekki við</t>
-  </si>
-  <si>
-    <t>karlkyn</t>
-  </si>
-  <si>
-    <t>Fullkomin</t>
-  </si>
-  <si>
-    <t>Hefu aðgang að öllu</t>
-  </si>
-  <si>
-    <t>His brain</t>
-  </si>
-  <si>
-    <t>allstaðar</t>
-  </si>
-  <si>
-    <t>Sá mikilvægasti</t>
+    <t>Þar sem nettenging finnst</t>
+  </si>
+  <si>
+    <t>Reynslu og góða þekkingu</t>
+  </si>
+  <si>
+    <t>Yfirmenn sem þurfa að fá upplýsingar úr kerfinu</t>
+  </si>
+  <si>
+    <t>Aðrir yfirmenn</t>
+  </si>
+  <si>
+    <t>Mjög mikilvægir</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5 - 13</t>
   </si>
 </sst>
 </file>
@@ -518,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -629,9 +620,12 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -914,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -925,19 +919,18 @@
     <col min="1" max="1" width="35.453125" style="3" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="31.453125" customWidth="1"/>
-    <col min="4" max="4" width="29.453125" customWidth="1"/>
-    <col min="5" max="5" width="33.81640625" customWidth="1"/>
+    <col min="4" max="4" width="33.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -945,23 +938,21 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
-    </row>
-    <row r="5" spans="1:5" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
@@ -971,12 +962,11 @@
       <c r="C5" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="34"/>
-    </row>
-    <row r="6" spans="1:5" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
         <v>3</v>
       </c>
@@ -986,12 +976,11 @@
       <c r="C6" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
         <v>4</v>
       </c>
@@ -1001,12 +990,11 @@
       <c r="C7" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
@@ -1016,130 +1004,121 @@
       <c r="C8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="23"/>
-    </row>
-    <row r="10" spans="1:5" ht="171" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="171" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="40" t="s">
-        <v>23</v>
+      <c r="B10" s="38" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="24">
-        <v>1</v>
-      </c>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-    </row>
-    <row r="12" spans="1:5" ht="103" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D11" s="27"/>
+    </row>
+    <row r="12" spans="1:4" ht="103" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="6"/>
       <c r="B12" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="25"/>
-    </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" s="11" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D13" s="27"/>
+    </row>
+    <row r="14" spans="1:4" s="11" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10"/>
       <c r="B14" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="36"/>
-    </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
-    </row>
-    <row r="16" spans="1:5" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="1:4" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-    </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-    </row>
-    <row r="18" spans="1:5" ht="67" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:4" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="21"/>
-    </row>
-    <row r="19" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>8</v>
       </c>
@@ -1149,12 +1128,11 @@
       <c r="C19" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="34"/>
-    </row>
-    <row r="20" spans="1:5" ht="63.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D19" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="63.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14" t="s">
         <v>9</v>
       </c>
@@ -1164,39 +1142,37 @@
       <c r="C20" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="21"/>
-    </row>
-    <row r="21" spans="1:5" ht="117.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D20" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="117.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="31"/>
-    </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
     </row>
-    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
     </row>
-    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
     </row>
-    <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
     </row>
-    <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
     </row>
   </sheetData>

</xml_diff>